<commit_message>
add he document creator modal in template // require ha document creator modal // require route setup in template-routes
</commit_message>
<xml_diff>
--- a/uploads/Weekly plan_SCM Customs_052020.xlsx
+++ b/uploads/Weekly plan_SCM Customs_052020.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\Team\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\junehyok.cho\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -329,18 +329,18 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -361,9 +361,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -401,7 +401,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
         <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -473,7 +473,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -650,57 +650,57 @@
   <dimension ref="A2:AE33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="U27" sqref="U27"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="28.85546875" customWidth="1"/>
     <col min="3" max="3" width="18.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:31" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15"/>
-      <c r="C2" s="15"/>
-      <c r="D2" s="16" t="s">
+      <c r="B2" s="16"/>
+      <c r="C2" s="16"/>
+      <c r="D2" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="15" t="s">
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+      <c r="G2" s="16"/>
+      <c r="H2" s="16"/>
+      <c r="I2" s="16"/>
+      <c r="J2" s="16"/>
+      <c r="K2" s="16" t="s">
         <v>6</v>
       </c>
-      <c r="L2" s="15"/>
-      <c r="M2" s="15"/>
-      <c r="N2" s="15"/>
-      <c r="O2" s="15"/>
-      <c r="P2" s="15"/>
-      <c r="Q2" s="15"/>
-      <c r="R2" s="15" t="s">
+      <c r="L2" s="16"/>
+      <c r="M2" s="16"/>
+      <c r="N2" s="16"/>
+      <c r="O2" s="16"/>
+      <c r="P2" s="16"/>
+      <c r="Q2" s="16"/>
+      <c r="R2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="15"/>
-      <c r="T2" s="15"/>
-      <c r="U2" s="15"/>
-      <c r="V2" s="15"/>
-      <c r="W2" s="15"/>
-      <c r="X2" s="15"/>
-      <c r="Y2" s="15" t="s">
+      <c r="S2" s="16"/>
+      <c r="T2" s="16"/>
+      <c r="U2" s="16"/>
+      <c r="V2" s="16"/>
+      <c r="W2" s="16"/>
+      <c r="X2" s="16"/>
+      <c r="Y2" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="Z2" s="15"/>
-      <c r="AA2" s="15"/>
-      <c r="AB2" s="15"/>
-      <c r="AC2" s="15"/>
-      <c r="AD2" s="15"/>
-      <c r="AE2" s="15"/>
+      <c r="Z2" s="16"/>
+      <c r="AA2" s="16"/>
+      <c r="AB2" s="16"/>
+      <c r="AC2" s="16"/>
+      <c r="AD2" s="16"/>
+      <c r="AE2" s="16"/>
     </row>
     <row r="3" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
@@ -798,7 +798,7 @@
       </c>
     </row>
     <row r="4" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="15" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -875,7 +875,7 @@
       <c r="AE4" s="5"/>
     </row>
     <row r="5" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="15" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="4" t="s">
@@ -952,7 +952,7 @@
       <c r="AE5" s="5"/>
     </row>
     <row r="6" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="15" t="s">
         <v>23</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -1029,7 +1029,7 @@
       <c r="AE6" s="5"/>
     </row>
     <row r="7" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="15" t="s">
         <v>24</v>
       </c>
       <c r="B7" s="4" t="s">
@@ -1106,7 +1106,7 @@
       <c r="AE7" s="5"/>
     </row>
     <row r="8" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A8" s="17" t="s">
+      <c r="A8" s="15" t="s">
         <v>25</v>
       </c>
       <c r="B8" s="4" t="s">
@@ -1183,7 +1183,7 @@
       <c r="AE8" s="5"/>
     </row>
     <row r="9" spans="1:31" ht="16.5" x14ac:dyDescent="0.3">
-      <c r="A9" s="17" t="s">
+      <c r="A9" s="15" t="s">
         <v>26</v>
       </c>
       <c r="B9" s="4" t="s">
@@ -1741,7 +1741,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1753,7 +1753,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>